<commit_message>
Updates to schedule and report
</commit_message>
<xml_diff>
--- a/Project Work Schedule.xlsx
+++ b/Project Work Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Proof of concept</t>
   </si>
@@ -75,9 +75,6 @@
 Select open source support, writeup for report.</t>
   </si>
   <si>
-    <t>Program drone to follow tag.</t>
-  </si>
-  <si>
     <t>Program drone to follow color.</t>
   </si>
   <si>
@@ -97,13 +94,47 @@
   <si>
     <t>Complete presentation.
 Deliver presentation.</t>
+  </si>
+  <si>
+    <t>Program drone to follow detection tag.</t>
+  </si>
+  <si>
+    <t>SW installs</t>
+  </si>
+  <si>
+    <t>Install the following tools in Linux box:
+  - Netbeans
+  - ROS
+  - Open CV
+  - AR Drone SDK</t>
+  </si>
+  <si>
+    <t>Tool integration references:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR Drone and ROS: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NetBeans and ROS: </t>
+  </si>
+  <si>
+    <t>http://wiki.ros.org/IDEs#NetBeans</t>
+  </si>
+  <si>
+    <t>http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-getting-started/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NetBeans and Open CV: </t>
+  </si>
+  <si>
+    <t>https://thefreecoder.wordpress.com/2012/09/10/use-netbeans-to-work-with-opencv-on-ubuntuand-linux-mint-and-other-distros-too/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +150,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -311,10 +350,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,11 +424,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -413,6 +527,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -441,126 +583,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -847,17 +870,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.140625" customWidth="1"/>
     <col min="5" max="6" width="20.7109375" style="1" customWidth="1"/>
   </cols>
@@ -867,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>2</v>
@@ -897,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="20" t="str">
-        <f ca="1">IF(F2="Yes","Yes",IF(A2&gt;TODAY(),"Yes",IF(A2=TODAY(),"Due today","No")))</f>
+        <f t="shared" ref="E2:E10" ca="1" si="0">IF(F2="Yes","Yes",IF(A2&gt;TODAY(),"Yes",IF(A2=TODAY(),"Due today","No")))</f>
         <v>Yes</v>
       </c>
       <c r="F2" s="21" t="s">
@@ -909,7 +932,7 @@
         <v>42308</v>
       </c>
       <c r="B3" s="7" t="str">
-        <f t="shared" ref="B3:B9" si="0">TEXT(A3,"dddd")</f>
+        <f t="shared" ref="B3:B10" si="1">TEXT(A3,"dddd")</f>
         <v>Saturday</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -919,73 +942,73 @@
         <v>14</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f ca="1">IF(F3="Yes","Yes",IF(A3&gt;TODAY(),"Yes",IF(A3=TODAY(),"Due today","No")))</f>
-        <v>Due today</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Yes</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
-        <v>42315</v>
+        <v>42310</v>
       </c>
       <c r="B4" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Saturday</v>
+        <f t="shared" si="1"/>
+        <v>Monday</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E4" s="4" t="str">
-        <f ca="1">IF(F4="Yes","Yes",IF(A4&gt;TODAY(),"Yes",IF(A4=TODAY(),"Due today","No")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
-        <v>42318</v>
+        <v>42315</v>
       </c>
       <c r="B5" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Tuesday</v>
+        <f t="shared" si="1"/>
+        <v>Saturday</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f ca="1">IF(F5="Yes","Yes",IF(A5&gt;TODAY(),"Yes",IF(A5=TODAY(),"Due today","No")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
-        <v>42325</v>
+        <v>42318</v>
       </c>
       <c r="B6" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f ca="1">IF(F6="Yes","Yes",IF(A6&gt;TODAY(),"Yes",IF(A6=TODAY(),"Due today","No")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -994,85 +1017,157 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
-        <v>42332</v>
+        <v>42325</v>
       </c>
       <c r="B7" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f ca="1">IF(F7="Yes","Yes",IF(A7&gt;TODAY(),"Yes",IF(A7=TODAY(),"Due today","No")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
-        <v>42353</v>
+        <v>42332</v>
       </c>
       <c r="B8" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f ca="1">IF(F8="Yes","Yes",IF(A8&gt;TODAY(),"Yes",IF(A8=TODAY(),"Due today","No")))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
         <v>42353</v>
       </c>
-      <c r="B9" s="12" t="str">
-        <f t="shared" si="0"/>
+      <c r="B9" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>42353</v>
+      </c>
+      <c r="B10" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="14" t="str">
-        <f ca="1">IF(F9="Yes","Yes",IF(A9&gt;TODAY(),"Yes",IF(A9=TODAY(),"Due today","No")))</f>
+      <c r="D10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:F12">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A2:F12 D14:D15 E13:F13 A13:C13 C16">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$F2="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>$E2="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F9">
-    <cfRule type="expression" dxfId="3" priority="2">
+  <conditionalFormatting sqref="A2:F10">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>$E2="Due today"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+      <formula>$F14="Yes"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>$E14="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>$F15="Yes"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$E15="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D15" r:id="rId1" location="NetBeans"/>
+    <hyperlink ref="D14" r:id="rId2"/>
+    <hyperlink ref="D16" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to report and schedule
</commit_message>
<xml_diff>
--- a/Project Work Schedule.xlsx
+++ b/Project Work Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Proof of concept</t>
   </si>
@@ -102,39 +102,73 @@
     <t>SW installs</t>
   </si>
   <si>
-    <t>Install the following tools in Linux box:
-  - Netbeans
-  - ROS
+    <t>Complete Robohub tutorials</t>
+  </si>
+  <si>
+    <t>Tutorials</t>
+  </si>
+  <si>
+    <t>1)  http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-getting-started/</t>
+  </si>
+  <si>
+    <t>2)  http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-joystick-control/</t>
+  </si>
+  <si>
+    <t>3)  http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-handling-feedback/</t>
+  </si>
+  <si>
+    <t>Install ardrone_autonomy package</t>
+  </si>
+  <si>
+    <t>https://svn.ardrone.org/boards/1/topics/show/5942</t>
+  </si>
+  <si>
+    <t>http://gauth.fr/2011/09/introduction-to-the-ar-drone-sdk/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Install the following tools in Linux box:
+  - </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Netbeans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  - Qt Creator - DONE
+  - ROS - Done
+  - Git - DONE
   - Open CV
-  - AR Drone SDK</t>
-  </si>
-  <si>
-    <t>Tool integration references:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR Drone and ROS: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NetBeans and ROS: </t>
-  </si>
-  <si>
-    <t>http://wiki.ros.org/IDEs#NetBeans</t>
-  </si>
-  <si>
-    <t>http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-getting-started/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NetBeans and Open CV: </t>
-  </si>
-  <si>
-    <t>https://thefreecoder.wordpress.com/2012/09/10/use-netbeans-to-work-with-opencv-on-ubuntuand-linux-mint-and-other-distros-too/</t>
+  - AR Drone SDK - DONE</t>
+    </r>
+  </si>
+  <si>
+    <t>Almost done w this one…</t>
+  </si>
+  <si>
+    <t>AR Drone SDK install help</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +192,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -425,14 +467,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -450,6 +501,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -492,6 +550,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -521,41 +586,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -870,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="20" t="str">
-        <f t="shared" ref="E2:E10" ca="1" si="0">IF(F2="Yes","Yes",IF(A2&gt;TODAY(),"Yes",IF(A2=TODAY(),"Due today","No")))</f>
+        <f t="shared" ref="E2:E12" ca="1" si="0">IF(F2="Yes","Yes",IF(A2&gt;TODAY(),"Yes",IF(A2=TODAY(),"Due today","No")))</f>
         <v>Yes</v>
       </c>
       <c r="F2" s="21" t="s">
@@ -932,7 +962,7 @@
         <v>42308</v>
       </c>
       <c r="B3" s="7" t="str">
-        <f t="shared" ref="B3:B10" si="1">TEXT(A3,"dddd")</f>
+        <f t="shared" ref="B3:B12" si="1">TEXT(A3,"dddd")</f>
         <v>Saturday</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -949,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>42310</v>
       </c>
@@ -961,11 +991,11 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>9</v>
@@ -976,80 +1006,80 @@
         <v>42315</v>
       </c>
       <c r="B5" s="7" t="str">
+        <f t="shared" ref="B5:B6" si="2">TEXT(A5,"dddd")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" ref="E5:E6" ca="1" si="3">IF(F5="Yes","Yes",IF(A5&gt;TODAY(),"Yes",IF(A5=TODAY(),"Due today","No")))</f>
+        <v>Due today</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>42315</v>
+      </c>
+      <c r="B6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Saturday</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>42315</v>
+      </c>
+      <c r="B7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Saturday</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>42318</v>
-      </c>
-      <c r="B6" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>42325</v>
-      </c>
-      <c r="B7" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>Tuesday</v>
-      </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Yes</v>
+        <v>Due today</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
-        <v>42332</v>
+        <v>42318</v>
       </c>
       <c r="B8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1059,19 +1089,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
-        <v>42353</v>
+        <v>42325</v>
       </c>
       <c r="B9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1081,93 +1111,159 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>42353</v>
-      </c>
-      <c r="B10" s="12" t="str">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>42332</v>
+      </c>
+      <c r="B10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Tuesday</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="14" t="str">
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>28</v>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>42353</v>
+      </c>
+      <c r="B11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>42353</v>
+      </c>
+      <c r="B12" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="28" t="s">
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="27" t="s">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="28"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="29" t="s">
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="28" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:F12 D14:D15 E13:F13 A13:C13 C16">
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="A2:F4 A7:F14 C15">
+    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
       <formula>$F2="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>$E2="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F10">
-    <cfRule type="expression" dxfId="10" priority="6">
+  <conditionalFormatting sqref="A2:F4 A7:F12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>$E2="Due today"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
-      <formula>$F14="Yes"</formula>
+  <conditionalFormatting sqref="A5:F5">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>$F5="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$E14="No"</formula>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$E5="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
-      <formula>$F15="Yes"</formula>
+  <conditionalFormatting sqref="A5:F5">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>$E5="Due today"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>$E15="No"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:F6">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>$F6="Yes"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$E6="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:F6">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$E6="Due today"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1" location="NetBeans"/>
-    <hyperlink ref="D14" r:id="rId2"/>
-    <hyperlink ref="D16" r:id="rId3"/>
+    <hyperlink ref="C16" r:id="rId1" display="http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-getting-started/"/>
+    <hyperlink ref="C17" r:id="rId2" display="http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-joystick-control/"/>
+    <hyperlink ref="C18" r:id="rId3" display="http://robohub.org/up-and-flying-with-the-ar-drone-and-ros-handling-feedback/"/>
+    <hyperlink ref="D20" r:id="rId4"/>
+    <hyperlink ref="D21" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>